<commit_message>
small fix in all templates
</commit_message>
<xml_diff>
--- a/fms_core/static/submission_templates/Container_creation_v0.3.xlsx
+++ b/fms_core/static/submission_templates/Container_creation_v0.3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kseni\Documents\fms\fms_core\static\submission_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5188065E-1109-44D1-A9D5-607E042A7E6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D3EEEC-D865-4D77-B610-914548C02F22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28560" yWindow="0" windowWidth="29040" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>